<commit_message>
diab incidence CIs added
</commit_message>
<xml_diff>
--- a/Data/diab_incidence.xlsx
+++ b/Data/diab_incidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\GitHub\NHANES_T2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\GitHub\NHANES_T2D\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Hispanic</t>
   </si>
@@ -40,13 +40,25 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>All_uCI</t>
+  </si>
+  <si>
+    <t>Hispanic_uCI</t>
+  </si>
+  <si>
+    <t>White_uCI</t>
+  </si>
+  <si>
+    <t>Black_uCI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -86,10 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,22 +383,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -393,413 +409,814 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2000</v>
       </c>
       <c r="B2" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="D2" s="2">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F2" s="2">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="3">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="H2" s="2">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I2" s="3">
+        <v>1.12E-2</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2001</v>
       </c>
       <c r="B3" s="2">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="3">
+        <v>1.1699999999999999E-2</v>
+      </c>
+      <c r="F3" s="2">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="3">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="H3" s="2">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I3" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2002</v>
       </c>
       <c r="B4" s="2">
         <v>7.0999999999999995E-3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="D4" s="2">
         <v>9.8000000000000014E-3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F4" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="3">
+        <v>6.9000000000000008E-3</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.01</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I4" s="3">
+        <v>1.21E-2</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2003</v>
       </c>
       <c r="B5" s="2">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="D5" s="2">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="3">
+        <v>1.1800000000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="3">
+        <v>6.9000000000000008E-3</v>
+      </c>
+      <c r="H5" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I5" s="3">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2004</v>
       </c>
       <c r="B6" s="2">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D6" s="2">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F6" s="2">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="3">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="H6" s="2">
         <v>1.03E-2</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I6" s="3">
+        <v>1.26E-2</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
       <c r="B7" s="2">
         <v>7.6E-3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
+        <v>8.199999999999999E-3</v>
+      </c>
+      <c r="D7" s="2">
         <v>1.01E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="3">
+        <v>1.21E-2</v>
+      </c>
+      <c r="F7" s="2">
         <v>6.6E-3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="G7" s="3">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="H7" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I7" s="3">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
       <c r="B8" s="2">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="D8" s="2">
         <v>9.6999999999999986E-3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F8" s="2">
         <v>6.9000000000000008E-3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="G8" s="3">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H8" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I8" s="3">
+        <v>1.24E-2</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
       <c r="B9" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D9" s="2">
         <v>1.09E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="3">
+        <v>1.3300000000000001E-2</v>
+      </c>
+      <c r="F9" s="2">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="E9" s="2">
+      <c r="G9" s="3">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="H9" s="2">
         <v>9.8000000000000014E-3</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I9" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
       <c r="B10" s="2">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="D10" s="2">
         <v>1.1900000000000001E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="3">
+        <v>1.43E-2</v>
+      </c>
+      <c r="F10" s="2">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="3">
+        <v>8.6E-3</v>
+      </c>
+      <c r="H10" s="2">
         <v>1.14E-2</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I10" s="3">
+        <v>1.52E-2</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
       <c r="B11" s="2">
         <v>8.4000000000000012E-3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="D11" s="2">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="3">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="F11" s="2">
         <v>7.1999999999999998E-3</v>
       </c>
-      <c r="E11" s="2">
+      <c r="G11" s="3">
+        <v>8.4000000000000012E-3</v>
+      </c>
+      <c r="H11" s="2">
         <v>1.1699999999999999E-2</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I11" s="3">
+        <v>1.55E-2</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
       <c r="B12" s="2">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D12" s="2">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="3">
+        <v>1.4199999999999999E-2</v>
+      </c>
+      <c r="F12" s="2">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="3">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H12" s="2">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I12" s="3">
+        <v>1.72E-2</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
       <c r="B13" s="2">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D13" s="2">
         <v>1.14E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F13" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E13" s="2">
+      <c r="G13" s="3">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="H13" s="2">
         <v>1.1699999999999999E-2</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="3">
+        <v>1.3800000000000002E-2</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
       <c r="B14" s="2">
         <v>7.0999999999999995E-3</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="D14" s="2">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="3">
+        <v>1.1800000000000001E-2</v>
+      </c>
+      <c r="F14" s="2">
         <v>6.0999999999999995E-3</v>
       </c>
-      <c r="E14" s="2">
+      <c r="G14" s="3">
+        <v>6.9000000000000008E-3</v>
+      </c>
+      <c r="H14" s="2">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I14" s="3">
+        <v>1.2199999999999999E-2</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2013</v>
       </c>
       <c r="B15" s="2">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D15" s="2">
         <v>9.6999999999999986E-3</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="3">
+        <v>1.15E-2</v>
+      </c>
+      <c r="F15" s="2">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="E15" s="2">
+      <c r="G15" s="3">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="H15" s="2">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I15" s="3">
+        <v>1.03E-2</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
       <c r="B16" s="2">
         <v>6.6E-3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="D16" s="2">
         <v>8.4000000000000012E-3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="3">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="F16" s="2">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="E16" s="2">
+      <c r="G16" s="3">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="H16" s="2">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I16" s="3">
+        <v>1.09E-2</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2015</v>
       </c>
       <c r="B17" s="2">
         <v>6.6E-3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="D17" s="2">
         <v>9.6999999999999986E-3</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="3">
+        <v>1.1699999999999999E-2</v>
+      </c>
+      <c r="F17" s="2">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="E17" s="2">
+      <c r="G17" s="3">
+        <v>6.3E-3</v>
+      </c>
+      <c r="H17" s="2">
         <v>9.8000000000000014E-3</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I17" s="3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2016</v>
       </c>
       <c r="B18" s="2">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
+        <v>7.0999999999999995E-3</v>
+      </c>
+      <c r="D18" s="2">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="3">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="F18" s="2">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E18" s="2">
+      <c r="G18" s="3">
+        <v>5.9000000000000007E-3</v>
+      </c>
+      <c r="H18" s="2">
         <v>9.8000000000000014E-3</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I18" s="3">
+        <v>1.2199999999999999E-2</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2017</v>
       </c>
       <c r="B19" s="2">
         <v>6.6E-3</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D19" s="2">
         <v>1.03E-2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="3">
+        <v>1.35E-2</v>
+      </c>
+      <c r="F19" s="2">
         <v>5.3E-3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="G19" s="3">
+        <v>6.0999999999999995E-3</v>
+      </c>
+      <c r="H19" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I19" s="3">
+        <v>1.12E-2</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2018</v>
       </c>
       <c r="B20" s="2">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D20" s="2">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="3">
+        <v>1.44E-2</v>
+      </c>
+      <c r="F20" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="G20" s="3">
+        <v>5.9000000000000007E-3</v>
+      </c>
+      <c r="H20" s="2">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>